<commit_message>
older version deleted - uploading updated files
</commit_message>
<xml_diff>
--- a/MultiHost/MeetingDetails.xlsx
+++ b/MultiHost/MeetingDetails.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MeetingName</t>
   </si>
@@ -27,21 +27,6 @@
   </si>
   <si>
     <t>MeetingStatus</t>
-  </si>
-  <si>
-    <t>LoadTest1</t>
-  </si>
-  <si>
-    <t>HostLoadTest1</t>
-  </si>
-  <si>
-    <t>192.168.43.146</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -109,23 +94,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>